<commit_message>
Added terminal blocks to BOM
</commit_message>
<xml_diff>
--- a/versions/V1p1/gerbers/BOM 6_Pack_V1p1.xlsx
+++ b/versions/V1p1/gerbers/BOM 6_Pack_V1p1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
   <si>
     <t>RefDes</t>
   </si>
@@ -373,7 +373,28 @@
     <t>TB1</t>
   </si>
   <si>
+    <t>2 Pos Terminal Block</t>
+  </si>
+  <si>
+    <t>Ningbo Xinlaiya Elec.</t>
+  </si>
+  <si>
+    <t>XY2500R-B-5.00-2P</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Pluggable-System-Terminal-Block_Ningbo-Xinlaiya-Elec-XY2500R-B-5-00-2P_C505815.html</t>
+  </si>
+  <si>
     <t>TB2, TB3, TB4, TB5, TB6, TB7</t>
+  </si>
+  <si>
+    <t>4 Pos Terminal Block</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Phoenix-Contact/1945119?qs=BYlwlsDsB%2FoxVFDUDE1oIQ%3D%3D</t>
   </si>
   <si>
     <t>U1</t>
@@ -413,7 +434,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -448,12 +469,8 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,12 +487,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -499,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -537,13 +548,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -572,6 +576,7 @@
     <col customWidth="1" min="3" max="4" width="10.0"/>
     <col customWidth="1" min="5" max="5" width="33.71"/>
     <col customWidth="1" min="7" max="7" width="23.43"/>
+    <col customWidth="1" min="8" max="8" width="28.57"/>
     <col customWidth="1" min="9" max="9" width="462.57"/>
   </cols>
   <sheetData>
@@ -1196,78 +1201,54 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="3">
         <v>0.0</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14"/>
-      <c r="Y24" s="14"/>
-      <c r="Z24" s="14"/>
-      <c r="AA24" s="14"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="14"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="14"/>
-      <c r="Z25" s="14"/>
-      <c r="AA25" s="14"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H25" s="4">
+        <v>1945119.0</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B26" s="3">
         <v>1.0</v>
@@ -1277,24 +1258,24 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B27" s="3">
         <v>4.0</v>
@@ -1304,36 +1285,36 @@
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" s="16">
+        <v>138</v>
+      </c>
+      <c r="B29" s="13">
         <f t="shared" ref="B29:D29" si="1">SUM(B4:B27)</f>
-        <v>64</v>
-      </c>
-      <c r="C29" s="16">
+        <v>65</v>
+      </c>
+      <c r="C29" s="13">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="13">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1359,9 +1340,11 @@
     <hyperlink r:id="rId19" ref="I21"/>
     <hyperlink r:id="rId20" ref="I22"/>
     <hyperlink r:id="rId21" ref="I23"/>
-    <hyperlink r:id="rId22" ref="I26"/>
-    <hyperlink r:id="rId23" ref="I27"/>
+    <hyperlink r:id="rId22" ref="I24"/>
+    <hyperlink r:id="rId23" ref="I25"/>
+    <hyperlink r:id="rId24" ref="I26"/>
+    <hyperlink r:id="rId25" ref="I27"/>
   </hyperlinks>
-  <drawing r:id="rId24"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>